<commit_message>
Correccion de estado de resultado
Corregido y verificado Estado de resultado
</commit_message>
<xml_diff>
--- a/catalogo_cuentas.xlsx
+++ b/catalogo_cuentas.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b7fb69822eb41239/Documents/NetBeansProjects/Estados-financieros/Estados-financieros/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="53" documentId="11_FFC65FC0516929C052170B45CB12EB475FEEECB1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7980C483-6A91-45D1-8AC4-41EBB6BF9582}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9430" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="136">
   <si>
     <t>Código</t>
   </si>
@@ -31,30 +37,84 @@
     <t>1002</t>
   </si>
   <si>
+    <t>1003</t>
+  </si>
+  <si>
     <t>1010</t>
   </si>
   <si>
     <t>1020</t>
   </si>
   <si>
+    <t>1030</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>1102</t>
+  </si>
+  <si>
+    <t>1201</t>
+  </si>
+  <si>
+    <t>1202</t>
+  </si>
+  <si>
+    <t>1301</t>
+  </si>
+  <si>
+    <t>1401</t>
+  </si>
+  <si>
     <t>2001</t>
   </si>
   <si>
     <t>2002</t>
   </si>
   <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2101</t>
+  </si>
+  <si>
+    <t>2102</t>
+  </si>
+  <si>
+    <t>2201</t>
+  </si>
+  <si>
+    <t>2301</t>
+  </si>
+  <si>
     <t>3001</t>
   </si>
   <si>
     <t>3002</t>
   </si>
   <si>
-    <t>4001</t>
+    <t>3003</t>
+  </si>
+  <si>
+    <t>3101</t>
+  </si>
+  <si>
+    <t>3102</t>
   </si>
   <si>
     <t>4002</t>
   </si>
   <si>
+    <t>4003</t>
+  </si>
+  <si>
+    <t>4101</t>
+  </si>
+  <si>
+    <t>4102</t>
+  </si>
+  <si>
     <t>5001</t>
   </si>
   <si>
@@ -64,43 +124,211 @@
     <t>5003</t>
   </si>
   <si>
+    <t>5004</t>
+  </si>
+  <si>
+    <t>5101</t>
+  </si>
+  <si>
+    <t>5102</t>
+  </si>
+  <si>
+    <t>5103</t>
+  </si>
+  <si>
+    <t>6001</t>
+  </si>
+  <si>
+    <t>6002</t>
+  </si>
+  <si>
+    <t>6003</t>
+  </si>
+  <si>
+    <t>6004</t>
+  </si>
+  <si>
+    <t>6005</t>
+  </si>
+  <si>
+    <t>6006</t>
+  </si>
+  <si>
+    <t>6007</t>
+  </si>
+  <si>
+    <t>6008</t>
+  </si>
+  <si>
+    <t>6009</t>
+  </si>
+  <si>
+    <t>6010</t>
+  </si>
+  <si>
+    <t>6011</t>
+  </si>
+  <si>
+    <t>7001</t>
+  </si>
+  <si>
+    <t>7002</t>
+  </si>
+  <si>
+    <t>7004</t>
+  </si>
+  <si>
+    <t>7005</t>
+  </si>
+  <si>
+    <t>8002</t>
+  </si>
+  <si>
+    <t>8003</t>
+  </si>
+  <si>
+    <t>8004</t>
+  </si>
+  <si>
     <t>Caja</t>
   </si>
   <si>
     <t>Bancos</t>
   </si>
   <si>
+    <t>Bancos en Inversiones</t>
+  </si>
+  <si>
     <t>Clientes</t>
   </si>
   <si>
     <t>Inventarios</t>
   </si>
   <si>
+    <t>Almacén</t>
+  </si>
+  <si>
+    <t>Documentos por cobrar</t>
+  </si>
+  <si>
+    <t>Deudores diversos</t>
+  </si>
+  <si>
+    <t>Mobiliario y equipo</t>
+  </si>
+  <si>
+    <t>Equipo de cómputo</t>
+  </si>
+  <si>
+    <t>Terrenos</t>
+  </si>
+  <si>
+    <t>Edificios</t>
+  </si>
+  <si>
     <t>Proveedores</t>
   </si>
   <si>
-    <t>Acreedores Diversos</t>
-  </si>
-  <si>
-    <t>Capital Social</t>
-  </si>
-  <si>
-    <t>Utilidades Retenidas</t>
+    <t>Acreedores diversos</t>
+  </si>
+  <si>
+    <t>Documentos por pagar</t>
+  </si>
+  <si>
+    <t>Impuestos por pagar</t>
+  </si>
+  <si>
+    <t>Sueldos por pagar</t>
+  </si>
+  <si>
+    <t>Préstamos bancarios CP</t>
+  </si>
+  <si>
+    <t>Préstamos bancarios LP</t>
+  </si>
+  <si>
+    <t>Capital social</t>
+  </si>
+  <si>
+    <t>Utilidades retenidas</t>
+  </si>
+  <si>
+    <t>Reserva legal</t>
+  </si>
+  <si>
+    <t>Utilidad del ejercicio</t>
+  </si>
+  <si>
+    <t>Pérdida del ejercicio</t>
   </si>
   <si>
     <t>Ventas</t>
   </si>
   <si>
+    <t>Ventas Totales</t>
+  </si>
+  <si>
     <t>Servicios Profesionales</t>
   </si>
   <si>
-    <t>Sueldos y Salarios</t>
-  </si>
-  <si>
-    <t>Renta de Oficina</t>
-  </si>
-  <si>
-    <t>Publicidad</t>
+    <t>Devoluciones sobre ventas</t>
+  </si>
+  <si>
+    <t>Descuentos sobre ventas</t>
+  </si>
+  <si>
+    <t>Inventario inicial</t>
+  </si>
+  <si>
+    <t>Inventario final</t>
+  </si>
+  <si>
+    <t>Compras</t>
+  </si>
+  <si>
+    <t>Devoluciones sobre compras</t>
+  </si>
+  <si>
+    <t>Descuentos sobre compras</t>
+  </si>
+  <si>
+    <t>Gastos de compra</t>
+  </si>
+  <si>
+    <t>Fletes y acarreos</t>
+  </si>
+  <si>
+    <t>Gastos de envío de mercancías</t>
+  </si>
+  <si>
+    <t>Sueldos del personal de ventas</t>
+  </si>
+  <si>
+    <t>Sueldos del personal de oficinas</t>
+  </si>
+  <si>
+    <t>Sueldos del chofer del equipo de reparto</t>
+  </si>
+  <si>
+    <t>Renta del almacén</t>
+  </si>
+  <si>
+    <t>Renta de oficinas</t>
+  </si>
+  <si>
+    <t>Intereses pagados</t>
+  </si>
+  <si>
+    <t>Intereses cobrados</t>
+  </si>
+  <si>
+    <t>Pérdida en cambios</t>
+  </si>
+  <si>
+    <t>Cambios ganados</t>
+  </si>
+  <si>
+    <t>Otros productos</t>
   </si>
   <si>
     <t>Activo</t>
@@ -116,13 +344,97 @@
   </si>
   <si>
     <t>Gasto</t>
+  </si>
+  <si>
+    <t>Mercancia</t>
+  </si>
+  <si>
+    <t>Equipo de oficina</t>
+  </si>
+  <si>
+    <t>1021</t>
+  </si>
+  <si>
+    <t>1203</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>Ventas – Deducciones</t>
+  </si>
+  <si>
+    <t>Costo de ventas</t>
+  </si>
+  <si>
+    <t>Gastos de venta</t>
+  </si>
+  <si>
+    <t>Propaganda y publicidad</t>
+  </si>
+  <si>
+    <t>Comisiones de agentes</t>
+  </si>
+  <si>
+    <t>Consumo de luz del almacén</t>
+  </si>
+  <si>
+    <t>Gastos de administración</t>
+  </si>
+  <si>
+    <t>Papelería y útiles</t>
+  </si>
+  <si>
+    <t>Consumo de luz de oficinas</t>
+  </si>
+  <si>
+    <t>Sueldos de agentes y dependientes</t>
+  </si>
+  <si>
+    <t>Gastos financieros</t>
+  </si>
+  <si>
+    <t>Productos financieros</t>
+  </si>
+  <si>
+    <t>Pérdida en venta de mobiliario</t>
+  </si>
+  <si>
+    <t>Otros gastos</t>
+  </si>
+  <si>
+    <t>Comisiones cobradas</t>
+  </si>
+  <si>
+    <t>8005</t>
+  </si>
+  <si>
+    <t>Consumo de luz de almacen</t>
+  </si>
+  <si>
+    <t>8006</t>
+  </si>
+  <si>
+    <t>Perdida</t>
+  </si>
+  <si>
+    <t>8007</t>
+  </si>
+  <si>
+    <t>Perdida en venta de acciones</t>
+  </si>
+  <si>
+    <t>8008</t>
+  </si>
+  <si>
+    <t>Dividendos cobrados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +446,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,13 +503,25 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -229,7 +559,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -263,6 +593,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -297,9 +628,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -472,14 +804,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="33.7265625" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,151 +827,760 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
+      <c r="B34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>122</v>
+      </c>
+      <c r="C49" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" t="s">
+        <v>106</v>
+      </c>
+      <c r="D53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" t="s">
+        <v>106</v>
+      </c>
+      <c r="D54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C55" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>128</v>
+      </c>
+      <c r="B57" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>132</v>
+      </c>
+      <c r="B59" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" t="s">
+        <v>107</v>
+      </c>
+      <c r="D59" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>134</v>
+      </c>
+      <c r="B60" t="s">
+        <v>135</v>
+      </c>
+      <c r="C60" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correccion del estado de resultado
Se corrigio el formato cuenta
</commit_message>
<xml_diff>
--- a/catalogo_cuentas.xlsx
+++ b/catalogo_cuentas.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="53" documentId="11_FFC65FC0516929C052170B45CB12EB475FEEECB1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7980C483-6A91-45D1-8AC4-41EBB6BF9582}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9430" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>